<commit_message>
Reverse words in a string
</commit_message>
<xml_diff>
--- a/C++/4.Array_Strings_Recursion_BackTracking/LC.xlsx
+++ b/C++/4.Array_Strings_Recursion_BackTracking/LC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/802969a580a30f56/Desktop/DS_ALGO/C^M^M/4.Array_Strings_Recursion_BackTracking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="11_F25DC773A252ABDACC104817091B6F3C5BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07F3D7D2-6D0A-45E8-A809-B9BD2EA06090}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="11_F25DC773A252ABDACC104817091B6F3C5BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0F02E7E-863B-483C-89C2-81D922657DFA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Topic Tags</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Array, Two Pointer, Recursion</t>
-  </si>
-  <si>
     <t>Array</t>
   </si>
   <si>
@@ -49,6 +46,30 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/print-words-vertically/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/two-sum/</t>
+  </si>
+  <si>
+    <t>Array, Hashmap</t>
+  </si>
+  <si>
+    <t>Solved using BruteForce. Can be improved</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-words-in-a-string/</t>
+  </si>
+  <si>
+    <t>Tokenize the string and reverse</t>
+  </si>
+  <si>
+    <t>Array, String</t>
+  </si>
+  <si>
+    <t>Array, Two Pointer, Recursion, String</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/rotate-array/</t>
   </si>
 </sst>
 </file>
@@ -418,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -448,68 +469,100 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{7E090650-01F6-4D14-B9F9-2345292142C8}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{ACA2D632-E61F-4572-AD67-548C14C78FA1}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{C5427D33-E681-4ECA-A799-132F18C89F05}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Using bit manipulation for subset & Subsequence
</commit_message>
<xml_diff>
--- a/C++/4.Array_Strings_Recursion_BackTracking/LC.xlsx
+++ b/C++/4.Array_Strings_Recursion_BackTracking/LC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/802969a580a30f56/Desktop/DS_ALGO/C^M^M/4.Array_Strings_Recursion_BackTracking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="11_F25DC773A252ABDACC104817091B6F3C5BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8EA2C0F-9ACF-4958-8212-91D68F955327}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="11_F25DC773A252ABDACC104817091B6F3C5BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A11B53F1-AC5F-41A0-9087-0D766353F8DD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Topic Tags</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>TLE if we use recursive way of generating subsequences</t>
+  </si>
+  <si>
+    <t>2^n recursive solution working</t>
   </si>
 </sst>
 </file>
@@ -484,7 +487,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -655,6 +658,10 @@
       <c r="B20" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="3"/>
     </row>
     <row r="22" spans="1:4">
       <c r="B22" s="2"/>

</xml_diff>